<commit_message>
fix: fixed tests and removed usage of measure specific parameters excel sheet
</commit_message>
<xml_diff>
--- a/import/raw_data/id_parameter.xlsx
+++ b/import/raw_data/id_parameter.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenz/Projekte/micat/import/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F5074E-D8D8-AC40-809C-242ECEC363B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DB1A08-73FC-FF48-A7D9-BA40EC5913BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="16780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="125">
   <si>
     <t>id</t>
   </si>
@@ -400,9 +400,6 @@
   </si>
   <si>
     <t>Damp and mouldy building target</t>
-  </si>
-  <si>
-    <t>Morbidity_AP</t>
   </si>
 </sst>
 </file>
@@ -739,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C65"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1456,14 +1453,6 @@
         <v>121</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65">
-        <v>64</v>
-      </c>
-      <c r="B65" t="s">
-        <v>125</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1471,18 +1460,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="89bcd336-abeb-4a08-b6b9-8f1906e00f8a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca47701c-f272-4f81-9665-1c7dbebc0776">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Type xmlns="ca47701c-f272-4f81-9665-1c7dbebc0776">id_table</Type>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010081027A5C4AB68A40A5017F28CDCC410C" ma:contentTypeVersion="17" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="f1f428d4bdb6f67b400b210b48125618">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ca47701c-f272-4f81-9665-1c7dbebc0776" xmlns:ns3="89bcd336-abeb-4a08-b6b9-8f1906e00f8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8189f6f0f7c839d9d0d3622fd62ec189" ns2:_="" ns3:_="">
     <xsd:import namespace="ca47701c-f272-4f81-9665-1c7dbebc0776"/>
@@ -1735,6 +1712,18 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="89bcd336-abeb-4a08-b6b9-8f1906e00f8a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca47701c-f272-4f81-9665-1c7dbebc0776">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Type xmlns="ca47701c-f272-4f81-9665-1c7dbebc0776">id_table</Type>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1745,17 +1734,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48414B01-8005-4D99-8041-3C881D221FD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="89bcd336-abeb-4a08-b6b9-8f1906e00f8a"/>
-    <ds:schemaRef ds:uri="ca47701c-f272-4f81-9665-1c7dbebc0776"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABFDCFC1-0950-4DFE-9D9B-4AF680B2B273}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1774,6 +1752,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48414B01-8005-4D99-8041-3C881D221FD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="89bcd336-abeb-4a08-b6b9-8f1906e00f8a"/>
+    <ds:schemaRef ds:uri="ca47701c-f272-4f81-9665-1c7dbebc0776"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8500D24-9B3E-4E37-8AAD-EB7D9C788023}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Added data for RES extension & updated doc on FEC-to-PEC conversion
</commit_message>
<xml_diff>
--- a/import/raw_data/id_parameter.xlsx
+++ b/import/raw_data/id_parameter.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bef\GitHub\micat\import\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B54CA0-1835-40D4-AE56-C13E7CFF8565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A79ECD6-EEA9-431F-8088-33C555F76FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27876" yWindow="2928" windowWidth="14400" windowHeight="8172" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="768" yWindow="768" windowWidth="46080" windowHeight="12072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="139">
   <si>
     <t>id</t>
   </si>
@@ -412,6 +423,36 @@
   </si>
   <si>
     <t>Conversion efficiency factors for electricity and heat power plants, as well as hydrogen production</t>
+  </si>
+  <si>
+    <t>RES energy allocation</t>
+  </si>
+  <si>
+    <t>Generated final energy carrier and necessary quantity of final energy carriers for the generation</t>
+  </si>
+  <si>
+    <t>Substitution factors</t>
+  </si>
+  <si>
+    <t>Coefficients specifying substituted electricity generators for each renewable electricity technology</t>
+  </si>
+  <si>
+    <t>Running costs</t>
+  </si>
+  <si>
+    <t>Variable running costs</t>
+  </si>
+  <si>
+    <t>Investment costs per capacity</t>
+  </si>
+  <si>
+    <t>Capital costs depending on installed capacity (CAPEX)</t>
+  </si>
+  <si>
+    <t>Running costs depending on installed capacity in M€/MW (OPEX)</t>
+  </si>
+  <si>
+    <t>Running costs depending on generated energy in M€/MWh (OPEX)</t>
   </si>
 </sst>
 </file>
@@ -748,20 +789,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.453125" customWidth="1"/>
-    <col min="2" max="2" width="36.08984375" customWidth="1"/>
-    <col min="3" max="3" width="93.36328125" customWidth="1"/>
+    <col min="1" max="1" width="5.44140625" customWidth="1"/>
+    <col min="2" max="2" width="36.109375" customWidth="1"/>
+    <col min="3" max="3" width="93.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -772,7 +813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -783,7 +824,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -794,7 +835,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -805,7 +846,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -816,7 +857,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -827,7 +868,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -838,7 +879,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -849,7 +890,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -860,7 +901,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -871,7 +912,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -882,7 +923,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -893,7 +934,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -904,7 +945,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -915,7 +956,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -926,7 +967,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -937,7 +978,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -948,7 +989,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -959,7 +1000,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -970,7 +1011,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -981,7 +1022,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -992,7 +1033,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1003,7 +1044,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1014,7 +1055,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1025,7 +1066,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1036,7 +1077,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1047,7 +1088,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1058,7 +1099,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1069,7 +1110,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1080,7 +1121,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1091,7 +1132,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1102,7 +1143,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1113,7 +1154,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1124,7 +1165,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1135,7 +1176,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1146,7 +1187,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1157,7 +1198,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1168,7 +1209,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1179,7 +1220,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1190,7 +1231,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1201,7 +1242,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1212,7 +1253,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1223,7 +1264,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1234,7 +1275,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1245,7 +1286,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1256,7 +1297,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1267,7 +1308,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1278,7 +1319,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1289,7 +1330,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1300,7 +1341,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1311,7 +1352,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1322,7 +1363,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1333,7 +1374,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1344,7 +1385,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1355,7 +1396,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1366,7 +1407,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1377,7 +1418,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1388,7 +1429,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1399,7 +1440,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1410,7 +1451,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1421,7 +1462,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1432,7 +1473,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1443,7 +1484,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1454,7 +1495,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1465,7 +1506,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1476,7 +1517,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1485,6 +1526,61 @@
       </c>
       <c r="C66" t="s">
         <v>128</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>129</v>
+      </c>
+      <c r="C67" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>131</v>
+      </c>
+      <c r="C68" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>135</v>
+      </c>
+      <c r="C69" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>133</v>
+      </c>
+      <c r="C70" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>134</v>
+      </c>
+      <c r="C71" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1494,15 +1590,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="89bcd336-abeb-4a08-b6b9-8f1906e00f8a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca47701c-f272-4f81-9665-1c7dbebc0776">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Type xmlns="ca47701c-f272-4f81-9665-1c7dbebc0776">id_table</Type>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1759,21 +1852,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="89bcd336-abeb-4a08-b6b9-8f1906e00f8a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca47701c-f272-4f81-9665-1c7dbebc0776">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Type xmlns="ca47701c-f272-4f81-9665-1c7dbebc0776">id_table</Type>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48414B01-8005-4D99-8041-3C881D221FD3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8500D24-9B3E-4E37-8AAD-EB7D9C788023}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="89bcd336-abeb-4a08-b6b9-8f1906e00f8a"/>
-    <ds:schemaRef ds:uri="ca47701c-f272-4f81-9665-1c7dbebc0776"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1798,9 +1891,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8500D24-9B3E-4E37-8AAD-EB7D9C788023}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48414B01-8005-4D99-8041-3C881D221FD3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="89bcd336-abeb-4a08-b6b9-8f1906e00f8a"/>
+    <ds:schemaRef ds:uri="ca47701c-f272-4f81-9665-1c7dbebc0776"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Data for Critical Raw material indicator
added raw data for the implementation of the new indicator on CRM
</commit_message>
<xml_diff>
--- a/import/raw_data/id_parameter.xlsx
+++ b/import/raw_data/id_parameter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bef\GitHub\micat\import\raw_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ren\Documents\GitHub\micat\import\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A79ECD6-EEA9-431F-8088-33C555F76FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246EA318-592E-49C2-A895-11D56F3087E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="768" yWindow="768" windowWidth="46080" windowHeight="12072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33945" yWindow="1995" windowWidth="33195" windowHeight="17670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="143">
   <si>
     <t>id</t>
   </si>
@@ -453,6 +453,18 @@
   </si>
   <si>
     <t>Running costs depending on generated energy in M€/MWh (OPEX)</t>
+  </si>
+  <si>
+    <t>Material intensity</t>
+  </si>
+  <si>
+    <t>Material intensity per MW installed capcity per technology in kg/MW</t>
+  </si>
+  <si>
+    <t>Supply risk factor</t>
+  </si>
+  <si>
+    <t>Supply risk factor per MW installed capcity per technology (unitless)</t>
   </si>
 </sst>
 </file>
@@ -511,7 +523,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -789,20 +801,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C71"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" customWidth="1"/>
-    <col min="2" max="2" width="36.109375" customWidth="1"/>
-    <col min="3" max="3" width="93.33203125" customWidth="1"/>
+    <col min="1" max="1" width="5.453125" customWidth="1"/>
+    <col min="2" max="2" width="36.08984375" customWidth="1"/>
+    <col min="3" max="3" width="93.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -813,7 +825,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -824,7 +836,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -835,7 +847,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -846,7 +858,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -857,7 +869,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -868,7 +880,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -879,7 +891,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -890,7 +902,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -901,7 +913,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -912,7 +924,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -923,7 +935,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -934,7 +946,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -945,7 +957,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -956,7 +968,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -967,7 +979,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -978,7 +990,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -989,7 +1001,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1000,7 +1012,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1011,7 +1023,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1022,7 +1034,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1033,7 +1045,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1044,7 +1056,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1055,7 +1067,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1066,7 +1078,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1077,7 +1089,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1088,7 +1100,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1099,7 +1111,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1110,7 +1122,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1121,7 +1133,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1132,7 +1144,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1143,7 +1155,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1154,7 +1166,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1165,7 +1177,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1176,7 +1188,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1187,7 +1199,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1198,7 +1210,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1209,7 +1221,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1220,7 +1232,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1231,7 +1243,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1242,7 +1254,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1253,7 +1265,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1264,7 +1276,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1275,7 +1287,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1286,7 +1298,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1297,7 +1309,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1308,7 +1320,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1319,7 +1331,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1330,7 +1342,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1341,7 +1353,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1352,7 +1364,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1363,7 +1375,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1374,7 +1386,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1385,7 +1397,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1396,7 +1408,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1407,7 +1419,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1418,7 +1430,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1429,7 +1441,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1440,7 +1452,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1451,7 +1463,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1462,7 +1474,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1473,7 +1485,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1484,7 +1496,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1495,7 +1507,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1506,7 +1518,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1517,7 +1529,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1528,7 +1540,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>66</v>
       </c>
@@ -1539,7 +1551,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>67</v>
       </c>
@@ -1550,7 +1562,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>68</v>
       </c>
@@ -1561,7 +1573,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>69</v>
       </c>
@@ -1572,7 +1584,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>70</v>
       </c>
@@ -1581,6 +1593,28 @@
       </c>
       <c r="C71" t="s">
         <v>138</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>139</v>
+      </c>
+      <c r="C72" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>141</v>
+      </c>
+      <c r="C73" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1590,12 +1624,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="89bcd336-abeb-4a08-b6b9-8f1906e00f8a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca47701c-f272-4f81-9665-1c7dbebc0776">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Type xmlns="ca47701c-f272-4f81-9665-1c7dbebc0776">id_table</Type>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1852,21 +1889,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="89bcd336-abeb-4a08-b6b9-8f1906e00f8a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca47701c-f272-4f81-9665-1c7dbebc0776">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Type xmlns="ca47701c-f272-4f81-9665-1c7dbebc0776">id_table</Type>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8500D24-9B3E-4E37-8AAD-EB7D9C788023}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48414B01-8005-4D99-8041-3C881D221FD3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="89bcd336-abeb-4a08-b6b9-8f1906e00f8a"/>
+    <ds:schemaRef ds:uri="ca47701c-f272-4f81-9665-1c7dbebc0776"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1891,12 +1928,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48414B01-8005-4D99-8041-3C881D221FD3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8500D24-9B3E-4E37-8AAD-EB7D9C788023}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="89bcd336-abeb-4a08-b6b9-8f1906e00f8a"/>
-    <ds:schemaRef ds:uri="ca47701c-f272-4f81-9665-1c7dbebc0776"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
New data for indicator land use
Data for the RES indicator land use is provided to the raw data
</commit_message>
<xml_diff>
--- a/import/raw_data/id_parameter.xlsx
+++ b/import/raw_data/id_parameter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ren\Documents\GitHub\micat\import\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246EA318-592E-49C2-A895-11D56F3087E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E402BF5F-BA9E-411A-AE8C-B71F5E08A741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33945" yWindow="1995" windowWidth="33195" windowHeight="17670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="54960" yWindow="-3360" windowWidth="35865" windowHeight="19590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="147">
   <si>
     <t>id</t>
   </si>
@@ -465,6 +465,18 @@
   </si>
   <si>
     <t>Supply risk factor per MW installed capcity per technology (unitless)</t>
+  </si>
+  <si>
+    <t>Land use (conventional)</t>
+  </si>
+  <si>
+    <t>Land use (RES)</t>
+  </si>
+  <si>
+    <t>Land use per MWh produced electricity _fossil electricity generation (m2/MWh)</t>
+  </si>
+  <si>
+    <t>Land use per MWh produced electricity_renewable electricity generation (m2/MWh)</t>
   </si>
 </sst>
 </file>
@@ -801,10 +813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1617,6 +1629,28 @@
         <v>142</v>
       </c>
     </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>143</v>
+      </c>
+      <c r="C74" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>144</v>
+      </c>
+      <c r="C75" t="s">
+        <v>146</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1624,18 +1658,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="89bcd336-abeb-4a08-b6b9-8f1906e00f8a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca47701c-f272-4f81-9665-1c7dbebc0776">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Type xmlns="ca47701c-f272-4f81-9665-1c7dbebc0776">id_table</Type>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010081027A5C4AB68A40A5017F28CDCC410C" ma:contentTypeVersion="17" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="f1f428d4bdb6f67b400b210b48125618">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ca47701c-f272-4f81-9665-1c7dbebc0776" xmlns:ns3="89bcd336-abeb-4a08-b6b9-8f1906e00f8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8189f6f0f7c839d9d0d3622fd62ec189" ns2:_="" ns3:_="">
     <xsd:import namespace="ca47701c-f272-4f81-9665-1c7dbebc0776"/>
@@ -1888,6 +1910,18 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="89bcd336-abeb-4a08-b6b9-8f1906e00f8a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca47701c-f272-4f81-9665-1c7dbebc0776">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Type xmlns="ca47701c-f272-4f81-9665-1c7dbebc0776">id_table</Type>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1898,17 +1932,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48414B01-8005-4D99-8041-3C881D221FD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="89bcd336-abeb-4a08-b6b9-8f1906e00f8a"/>
-    <ds:schemaRef ds:uri="ca47701c-f272-4f81-9665-1c7dbebc0776"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABFDCFC1-0950-4DFE-9D9B-4AF680B2B273}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1927,6 +1950,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48414B01-8005-4D99-8041-3C881D221FD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="89bcd336-abeb-4a08-b6b9-8f1906e00f8a"/>
+    <ds:schemaRef ds:uri="ca47701c-f272-4f81-9665-1c7dbebc0776"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8500D24-9B3E-4E37-8AAD-EB7D9C788023}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Data and IDs for energy system cost
upload of extended ID parameter table and raw data for the new indicator
</commit_message>
<xml_diff>
--- a/import/raw_data/id_parameter.xlsx
+++ b/import/raw_data/id_parameter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ren\Documents\GitHub\micat\import\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E402BF5F-BA9E-411A-AE8C-B71F5E08A741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FE9922-70A4-4F14-B5CD-B5632C01553A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54960" yWindow="-3360" windowWidth="35865" windowHeight="19590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="52095" yWindow="2415" windowWidth="30555" windowHeight="17865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="151">
   <si>
     <t>id</t>
   </si>
@@ -477,6 +477,18 @@
   </si>
   <si>
     <t>Land use per MWh produced electricity_renewable electricity generation (m2/MWh)</t>
+  </si>
+  <si>
+    <t>VRE penetration</t>
+  </si>
+  <si>
+    <t>Energy System Cost</t>
+  </si>
+  <si>
+    <t>Variable Renewable Energy (VRE) penetration is defined as the share of wind and solar generation in annual gross electricity production</t>
+  </si>
+  <si>
+    <t>Total energy system costs including balancing, profile, and grid costs, associated with integrating VRE at different penetration levels. [€/MWh]</t>
   </si>
 </sst>
 </file>
@@ -813,10 +825,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C75"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1651,6 +1663,28 @@
         <v>146</v>
       </c>
     </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>147</v>
+      </c>
+      <c r="C76" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>148</v>
+      </c>
+      <c r="C77" t="s">
+        <v>150</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1658,6 +1692,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="89bcd336-abeb-4a08-b6b9-8f1906e00f8a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca47701c-f272-4f81-9665-1c7dbebc0776">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Type xmlns="ca47701c-f272-4f81-9665-1c7dbebc0776">id_table</Type>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010081027A5C4AB68A40A5017F28CDCC410C" ma:contentTypeVersion="17" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="f1f428d4bdb6f67b400b210b48125618">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ca47701c-f272-4f81-9665-1c7dbebc0776" xmlns:ns3="89bcd336-abeb-4a08-b6b9-8f1906e00f8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8189f6f0f7c839d9d0d3622fd62ec189" ns2:_="" ns3:_="">
     <xsd:import namespace="ca47701c-f272-4f81-9665-1c7dbebc0776"/>
@@ -1910,28 +1965,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="89bcd336-abeb-4a08-b6b9-8f1906e00f8a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca47701c-f272-4f81-9665-1c7dbebc0776">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Type xmlns="ca47701c-f272-4f81-9665-1c7dbebc0776">id_table</Type>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8500D24-9B3E-4E37-8AAD-EB7D9C788023}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48414B01-8005-4D99-8041-3C881D221FD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="89bcd336-abeb-4a08-b6b9-8f1906e00f8a"/>
+    <ds:schemaRef ds:uri="ca47701c-f272-4f81-9665-1c7dbebc0776"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABFDCFC1-0950-4DFE-9D9B-4AF680B2B273}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1948,23 +2001,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48414B01-8005-4D99-8041-3C881D221FD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="89bcd336-abeb-4a08-b6b9-8f1906e00f8a"/>
-    <ds:schemaRef ds:uri="ca47701c-f272-4f81-9665-1c7dbebc0776"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8500D24-9B3E-4E37-8AAD-EB7D9C788023}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>